<commit_message>
refactor: create federal_purchases_test data series
Proof of concept to re-create one of the 33 FIM input series using only basic source files (national accounts, forecast) for better clarity. Results plug into the contribution() function to produce federal_purchases_contribution
</commit_message>
<xml_diff>
--- a/docs/making sense of data imports.xlsx
+++ b/docs/making sense of data imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoja\dev\FIM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7605D928-FDAF-4463-8629-904AC90C9A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA0207B-9C89-40F4-A886-BB7F8A266FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3390" windowWidth="29040" windowHeight="15720" xr2:uid="{4D20AEA8-C2CB-4382-9050-4CBB9B5317F0}"/>
   </bookViews>
@@ -754,9 +754,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -769,6 +766,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,10 +785,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1110,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992756FF-DFDB-4E6B-BBA1-0D587761BCAE}">
   <dimension ref="B1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,10 +1169,10 @@
       <c r="E7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="69"/>
+      <c r="I7" s="78"/>
     </row>
     <row r="8" spans="2:14" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -1219,85 +1215,85 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="2:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="70" t="s">
+    <row r="9" spans="2:14" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="71" t="s">
+      <c r="H9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="71" t="s">
+      <c r="I9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="71" t="s">
+      <c r="J9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="71" t="s">
+      <c r="K9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="71" t="s">
+      <c r="L9" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="73" t="s">
+      <c r="M9" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="71" t="s">
+      <c r="N9" s="70" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="70" t="s">
+    <row r="10" spans="2:14" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="71" t="s">
+      <c r="E10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="71" t="s">
+      <c r="H10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="71" t="s">
+      <c r="I10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="J10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="71" t="s">
+      <c r="K10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="71" t="s">
+      <c r="L10" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="73" t="s">
+      <c r="M10" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="70" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1312,7 +1308,7 @@
       <c r="G11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="75" t="s">
+      <c r="H11" s="74" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="18" t="s">
@@ -1351,7 +1347,7 @@
       <c r="I12" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="75" t="s">
         <v>53</v>
       </c>
       <c r="K12" s="37" t="s">
@@ -1400,7 +1396,7 @@
       <c r="I14" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="77" t="s">
+      <c r="J14" s="76" t="s">
         <v>4</v>
       </c>
       <c r="K14" s="55" t="s">
@@ -1429,7 +1425,7 @@
       <c r="I15" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="78" t="s">
+      <c r="J15" s="77" t="s">
         <v>3</v>
       </c>
       <c r="K15" s="55" t="s">

</xml_diff>